<commit_message>
got logistic regression baseline, one cnn result
which is definitely not as good anymore, and doesn't really top logistic regression, unfortunately
</commit_message>
<xml_diff>
--- a/Alex Code/Results/02142019/Log.xlsx
+++ b/Alex Code/Results/02142019/Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexw\Documents\GitHub\ARMS\Alex Code\Results\02142019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57C109F-A8C1-41A5-8D3A-85570E3B1AA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69AA140-DFEE-455B-A7A6-4BA747E22411}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="17256" windowHeight="5568" xr2:uid="{0D2A33BD-CCA2-4AFD-99E7-7CC52817BFBE}"/>
+    <workbookView xWindow="3744" yWindow="0" windowWidth="17256" windowHeight="5568" xr2:uid="{0D2A33BD-CCA2-4AFD-99E7-7CC52817BFBE}"/>
   </bookViews>
   <sheets>
     <sheet name="LogReg" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Inv. Reg</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Validation</t>
   </si>
   <si>
-    <t>PENDING</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>Acc</t>
+  </si>
+  <si>
+    <t>Threshold</t>
   </si>
 </sst>
 </file>
@@ -413,133 +413,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C1855E-D6F5-4F06-86C1-916EB89D45FA}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>0.9</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.7833</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.88239999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.9</v>
       </c>
       <c r="B3">
+        <v>0.9</v>
+      </c>
+      <c r="C3">
         <v>0.76900000000000002</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.86760000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>0.9</v>
+      </c>
+      <c r="B4">
         <v>0.8</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.76300000000000001</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.89710000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>0.9</v>
+      </c>
+      <c r="B5">
         <v>0.7</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.79069999999999996</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.89710000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
+        <v>0.9</v>
+      </c>
+      <c r="B6">
         <v>0.6</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.76390000000000002</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.88239999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>0.9</v>
+      </c>
+      <c r="B7">
         <v>0.5</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.75929999999999997</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.91180000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>0.9</v>
+      </c>
+      <c r="B8">
         <v>0.4</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.78149999999999997</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.89710000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.95</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.91169999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.95</v>
+      </c>
+      <c r="B10">
+        <v>0.9</v>
+      </c>
+      <c r="C10">
+        <v>0.74439999999999995</v>
+      </c>
+      <c r="D10">
+        <v>0.86760000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.95</v>
+      </c>
+      <c r="B11">
+        <v>0.8</v>
+      </c>
+      <c r="C11">
+        <v>0.74439999999999995</v>
+      </c>
+      <c r="D11">
+        <v>0.89710000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.95</v>
+      </c>
+      <c r="B12">
+        <v>0.7</v>
+      </c>
+      <c r="C12">
+        <v>0.74629999999999996</v>
+      </c>
+      <c r="D12">
+        <v>0.85289999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.95</v>
+      </c>
+      <c r="B13">
+        <v>0.6</v>
+      </c>
+      <c r="C13">
+        <v>0.74070000000000003</v>
+      </c>
+      <c r="D13">
+        <v>0.89710000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0.95</v>
+      </c>
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+      <c r="C14">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="D14">
+        <v>0.88239999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
+        <v>0.9</v>
+      </c>
+      <c r="B20">
         <v>0.5</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>0.67859999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
       <c r="B21">
-        <v>0.72619999999999996</v>
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0.73809999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -549,10 +666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7194CBAD-476D-47B4-BFDA-604C4AEFAD3F}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,8 +725,11 @@
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
+      <c r="C5">
+        <v>0.80559999999999998</v>
+      </c>
+      <c r="D5">
+        <v>0.79410000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -619,58 +739,88 @@
       <c r="B6">
         <v>10</v>
       </c>
+      <c r="C6">
+        <v>0.87409999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.80879999999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>100</v>
+        <v>1500</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B8">
         <v>20</v>
       </c>
+      <c r="C8">
+        <v>0.79259999999999997</v>
+      </c>
+      <c r="D8">
+        <v>0.76470000000000005</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="B9">
         <v>20</v>
       </c>
+      <c r="C9">
+        <v>0.86851999999999996</v>
+      </c>
+      <c r="D9">
+        <v>0.92649999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>100</v>
+        <v>1500</v>
       </c>
       <c r="B10">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B11">
         <v>30</v>
       </c>
+      <c r="C11">
+        <v>0.79069999999999996</v>
+      </c>
+      <c r="D11">
+        <v>0.76470000000000005</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="B12">
         <v>30</v>
       </c>
+      <c r="C12">
+        <v>0.87222</v>
+      </c>
+      <c r="D12">
+        <v>0.91169999999999995</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="B13">
         <v>30</v>
@@ -678,50 +828,54 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>0.7944</v>
+      </c>
+      <c r="D14">
+        <v>0.79410000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B15">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>0.91849999999999998</v>
+      </c>
+      <c r="D15">
+        <v>0.94120000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="B16">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1000</v>
-      </c>
-      <c r="B17">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>1500</v>
-      </c>
-      <c r="B18">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>500</v>
+      </c>
+      <c r="B22">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>2000</v>
-      </c>
-      <c r="B19">
-        <v>50</v>
+      <c r="C22">
+        <v>0.72619999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results for combined filters experiment
</commit_message>
<xml_diff>
--- a/Alex Code/Results/02142019/Log.xlsx
+++ b/Alex Code/Results/02142019/Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexw\Documents\GitHub\ARMS\Alex Code\Results\02142019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512DC64E-7200-41B9-A378-6D498D89D617}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67072732-A407-4827-947D-1BFC75776FC0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3996" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{0D2A33BD-CCA2-4AFD-99E7-7CC52817BFBE}"/>
+    <workbookView xWindow="5376" yWindow="3048" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{0D2A33BD-CCA2-4AFD-99E7-7CC52817BFBE}"/>
   </bookViews>
   <sheets>
     <sheet name="LogReg" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Inv. Reg</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>PENDING3</t>
-  </si>
-  <si>
-    <t>Test Accuracy (shhhh)</t>
   </si>
   <si>
     <t>Dropout</t>
@@ -831,27 +828,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7194CBAD-476D-47B4-BFDA-604C4AEFAD3F}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="I14" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="8.88671875" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -868,11 +864,8 @@
       <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.95</v>
       </c>
@@ -889,7 +882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.95</v>
       </c>
@@ -906,7 +899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.95</v>
       </c>
@@ -923,7 +916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.95</v>
       </c>
@@ -940,7 +933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.95</v>
       </c>
@@ -960,7 +953,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.95</v>
       </c>
@@ -977,7 +970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.95</v>
       </c>
@@ -994,7 +987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.95</v>
       </c>
@@ -1011,7 +1004,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.95</v>
       </c>
@@ -1028,7 +1021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.95</v>
       </c>
@@ -1045,7 +1038,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.95</v>
       </c>
@@ -1070,11 +1063,8 @@
       <c r="H12">
         <v>0.91120000000000001</v>
       </c>
-      <c r="I12">
-        <v>0.63100000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.95</v>
       </c>
@@ -1099,11 +1089,8 @@
       <c r="H13">
         <v>0.92059999999999997</v>
       </c>
-      <c r="I13">
-        <v>0.65480000000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.95</v>
       </c>
@@ -1120,7 +1107,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0.95</v>
       </c>
@@ -1145,11 +1132,8 @@
       <c r="H15">
         <v>0.96499999999999997</v>
       </c>
-      <c r="I15">
-        <v>0.67859999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0.95</v>
       </c>
@@ -1174,11 +1158,8 @@
       <c r="H16">
         <v>0.97430000000000005</v>
       </c>
-      <c r="I16">
-        <v>0.67859999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0.95</v>
       </c>
@@ -1203,14 +1184,11 @@
       <c r="H17">
         <v>0.63319999999999999</v>
       </c>
-      <c r="I17">
-        <v>0.59519999999999995</v>
-      </c>
-      <c r="J17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0.95</v>
       </c>
@@ -1235,11 +1213,8 @@
       <c r="H18">
         <v>0.75229999999999997</v>
       </c>
-      <c r="I18">
-        <v>0.71430000000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0.95</v>
       </c>
@@ -1264,11 +1239,8 @@
       <c r="H19">
         <v>0.81779999999999997</v>
       </c>
-      <c r="I19">
-        <v>0.77380000000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0.95</v>
       </c>
@@ -1293,16 +1265,13 @@
       <c r="H20">
         <v>0.82010000000000005</v>
       </c>
-      <c r="I20">
-        <v>0.76190000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D22">
         <v>500</v>
       </c>
@@ -1310,7 +1279,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D23">
         <v>1000</v>
       </c>

</xml_diff>